<commit_message>
Fix Jinja2 template error, improve row numbering logic, and add email loading state
</commit_message>
<xml_diff>
--- a/EXCEL.xlsx
+++ b/EXCEL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAFIZI\iPetro_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAFIZI\OneDrive\Documents\Downloads\IPetro_Workshop_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD4EFDC8-D51D-4111-B72F-05A104212817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FDC012-162D-4C57-94DC-7E439850A1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{065ECA5C-B467-41B3-9273-2B8BDFD238BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{065ECA5C-B467-41B3-9273-2B8BDFD238BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">IPETRO PLANT </t>
   </si>
   <si>
     <t>MASTERFILE EQUIPMENT</t>
-  </si>
-  <si>
-    <t>TOTAL NO. OF EQUIPMENT: 10 EQUIPMENTS</t>
   </si>
   <si>
     <t>NO.</t>
@@ -263,55 +260,55 @@
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,125 +672,123 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" customWidth="1"/>
-    <col min="15" max="15" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="8"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="13" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="13" t="s">
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="13" t="s">
+      <c r="M7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="15"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="16"/>
-    </row>
-    <row r="7" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" s="18" t="s">
+      <c r="O7" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="O7" s="18" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>